<commit_message>
Moved call sign in EEPROM
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="1460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1461">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2243,6 +2243,9 @@
   </si>
   <si>
     <t xml:space="preserve">0x0F20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL SIGN</t>
   </si>
   <si>
     <t xml:space="preserve">0x0F30</t>
@@ -4656,11 +4659,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A206" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E236" activeCellId="0" sqref="E236"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A198" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B244" activeCellId="0" sqref="B244"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -12950,26 +12953,28 @@
       <c r="Y243" s="1"/>
       <c r="Z243" s="1"/>
     </row>
-    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="B244" s="5"/>
-      <c r="C244" s="5"/>
-      <c r="D244" s="5"/>
-      <c r="E244" s="5"/>
-      <c r="F244" s="5"/>
-      <c r="G244" s="5"/>
-      <c r="H244" s="5"/>
-      <c r="I244" s="5"/>
-      <c r="J244" s="5"/>
-      <c r="K244" s="5"/>
-      <c r="L244" s="5"/>
-      <c r="M244" s="5"/>
-      <c r="N244" s="5"/>
-      <c r="O244" s="5"/>
-      <c r="P244" s="5"/>
-      <c r="Q244" s="5"/>
+      <c r="B244" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
+      <c r="H244" s="3"/>
+      <c r="I244" s="3"/>
+      <c r="J244" s="3"/>
+      <c r="K244" s="3"/>
+      <c r="L244" s="3"/>
+      <c r="M244" s="3"/>
+      <c r="N244" s="3"/>
+      <c r="O244" s="3"/>
+      <c r="P244" s="3"/>
+      <c r="Q244" s="3"/>
       <c r="R244" s="1"/>
       <c r="S244" s="1"/>
       <c r="T244" s="1"/>
@@ -12982,10 +12987,10 @@
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
@@ -13014,28 +13019,28 @@
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="F246" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="G246" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="H246" s="4" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
@@ -13058,10 +13063,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13090,10 +13095,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13122,10 +13127,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13154,10 +13159,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13186,10 +13191,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13218,10 +13223,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13250,10 +13255,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13282,10 +13287,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13314,10 +13319,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13346,10 +13351,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13378,10 +13383,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13410,10 +13415,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13442,10 +13447,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13474,10 +13479,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13506,10 +13511,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13538,10 +13543,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13570,10 +13575,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13602,10 +13607,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13634,10 +13639,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13666,10 +13671,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13698,10 +13703,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13730,10 +13735,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13762,10 +13767,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13794,10 +13799,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13826,10 +13831,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13858,10 +13863,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13890,10 +13895,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13922,10 +13927,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -13954,10 +13959,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -13986,10 +13991,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -14018,10 +14023,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14050,10 +14055,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14082,10 +14087,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14114,10 +14119,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14146,10 +14151,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14178,10 +14183,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14210,10 +14215,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14242,10 +14247,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14274,10 +14279,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14306,10 +14311,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14338,10 +14343,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14370,10 +14375,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14402,10 +14407,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14434,10 +14439,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14466,10 +14471,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14498,10 +14503,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14530,10 +14535,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14562,10 +14567,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14594,10 +14599,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14626,10 +14631,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14658,10 +14663,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14690,10 +14695,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14722,10 +14727,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14754,10 +14759,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14786,10 +14791,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14818,10 +14823,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14850,10 +14855,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14882,10 +14887,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14914,10 +14919,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -14946,10 +14951,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -14978,10 +14983,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -15010,10 +15015,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15042,10 +15047,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15074,10 +15079,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15106,10 +15111,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15138,10 +15143,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15170,10 +15175,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15202,10 +15207,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15234,10 +15239,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15266,10 +15271,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15298,10 +15303,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15330,10 +15335,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15362,10 +15367,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15394,10 +15399,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15426,10 +15431,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15458,10 +15463,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15490,10 +15495,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15522,10 +15527,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15554,10 +15559,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15586,10 +15591,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15618,10 +15623,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15650,10 +15655,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15682,10 +15687,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15714,10 +15719,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15746,10 +15751,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15778,10 +15783,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15810,10 +15815,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15842,10 +15847,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15874,10 +15879,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15906,10 +15911,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15938,10 +15943,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -15970,10 +15975,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -16002,10 +16007,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -16034,10 +16039,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16066,10 +16071,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16098,10 +16103,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16130,10 +16135,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16162,10 +16167,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16194,10 +16199,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16226,10 +16231,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16258,10 +16263,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16290,10 +16295,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16322,10 +16327,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16354,10 +16359,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16386,10 +16391,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16418,10 +16423,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16450,10 +16455,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16482,10 +16487,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16514,10 +16519,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16546,10 +16551,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16578,10 +16583,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16610,10 +16615,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16642,10 +16647,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16674,10 +16679,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16706,10 +16711,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16738,10 +16743,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16770,10 +16775,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16802,10 +16807,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16834,10 +16839,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16866,10 +16871,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16898,10 +16903,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16930,10 +16935,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -16962,10 +16967,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -16994,10 +16999,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -17026,10 +17031,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17058,10 +17063,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17090,10 +17095,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17122,10 +17127,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17154,10 +17159,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17186,10 +17191,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17218,10 +17223,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17250,10 +17255,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17282,10 +17287,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17314,10 +17319,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17346,10 +17351,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17378,10 +17383,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17410,10 +17415,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17442,10 +17447,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17474,10 +17479,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17506,10 +17511,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17538,10 +17543,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17570,10 +17575,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17602,10 +17607,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17634,10 +17639,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17666,10 +17671,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17698,10 +17703,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17730,10 +17735,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17762,10 +17767,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17794,10 +17799,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17826,10 +17831,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17858,10 +17863,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17890,10 +17895,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17922,10 +17927,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -17954,10 +17959,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -17986,10 +17991,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -18018,10 +18023,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18050,10 +18055,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18082,10 +18087,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18114,10 +18119,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18146,10 +18151,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18178,10 +18183,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18210,10 +18215,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18242,10 +18247,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18274,10 +18279,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18306,10 +18311,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18338,10 +18343,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18370,10 +18375,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18402,10 +18407,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18434,10 +18439,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18466,10 +18471,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18498,10 +18503,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18530,10 +18535,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18562,10 +18567,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18594,10 +18599,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18626,10 +18631,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18658,10 +18663,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18690,10 +18695,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18722,10 +18727,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18754,10 +18759,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18786,10 +18791,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18818,10 +18823,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18850,10 +18855,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18882,10 +18887,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18914,10 +18919,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -18946,10 +18951,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -18978,10 +18983,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -19010,10 +19015,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19042,10 +19047,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19074,10 +19079,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19106,10 +19111,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19138,10 +19143,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19170,10 +19175,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19202,10 +19207,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19234,10 +19239,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19266,10 +19271,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19298,10 +19303,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19330,10 +19335,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19362,10 +19367,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19394,10 +19399,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19426,10 +19431,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19458,7 +19463,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19488,7 +19493,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19518,7 +19523,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19548,10 +19553,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19580,10 +19585,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19612,10 +19617,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19644,10 +19649,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19676,10 +19681,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19708,10 +19713,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19740,10 +19745,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19772,10 +19777,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19804,10 +19809,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19836,10 +19841,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19868,10 +19873,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19900,10 +19905,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19932,10 +19937,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -19964,10 +19969,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -19996,10 +20001,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -20028,10 +20033,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20060,7 +20065,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20090,7 +20095,7 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
@@ -20120,7 +20125,7 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
@@ -20150,7 +20155,7 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
@@ -20180,7 +20185,7 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
@@ -20210,7 +20215,7 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
@@ -20240,7 +20245,7 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
@@ -20270,7 +20275,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20300,7 +20305,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20330,7 +20335,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20360,7 +20365,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20390,7 +20395,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20420,7 +20425,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20450,7 +20455,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20480,7 +20485,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20510,7 +20515,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20548,7 +20553,7 @@
       <c r="G482" s="14"/>
       <c r="H482" s="14"/>
       <c r="I482" s="3" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="J482" s="3"/>
       <c r="K482" s="14"/>
@@ -20570,37 +20575,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20620,37 +20625,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20670,37 +20675,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20720,37 +20725,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20770,37 +20775,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20820,37 +20825,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20870,37 +20875,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20920,37 +20925,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -20970,37 +20975,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -21020,37 +21025,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21070,37 +21075,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21120,37 +21125,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21170,38 +21175,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21216,34 +21221,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21264,34 +21269,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21312,34 +21317,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21360,34 +21365,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21408,34 +21413,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21456,34 +21461,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21504,34 +21509,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21552,30 +21557,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21594,38 +21599,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21640,14 +21645,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21655,19 +21660,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21682,30 +21687,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21724,28 +21729,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21753,10 +21758,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21770,7 +21775,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21800,7 +21805,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21830,7 +21835,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21860,7 +21865,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21890,7 +21895,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21920,7 +21925,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21950,7 +21955,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>
@@ -35615,7 +35620,7 @@
       <c r="Z1001" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="498">
+  <mergeCells count="499">
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B3:Q3"/>
     <mergeCell ref="B4:Q4"/>
@@ -35861,6 +35866,7 @@
     <mergeCell ref="B242:I242"/>
     <mergeCell ref="J242:Q242"/>
     <mergeCell ref="B243:I243"/>
+    <mergeCell ref="B244:Q244"/>
     <mergeCell ref="B245:Q245"/>
     <mergeCell ref="B247:Q247"/>
     <mergeCell ref="B248:Q248"/>

</xml_diff>

<commit_message>
Added a Toggle for MURS while in FCC HAM
</commit_message>
<xml_diff>
--- a/docs/UV K5 EEPROM.xlsx
+++ b/docs/UV K5 EEPROM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="1462">
   <si>
     <t xml:space="preserve">00</t>
   </si>
@@ -2276,6 +2276,9 @@
   </si>
   <si>
     <t xml:space="preserve">SCRAMBLE_EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MURS TX</t>
   </si>
   <si>
     <t xml:space="preserve">0x0F50</t>
@@ -4659,11 +4662,11 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A198" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B244" activeCellId="0" sqref="B244"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A218" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I246" activeCellId="0" sqref="I246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -13017,7 +13020,7 @@
       <c r="Y245" s="1"/>
       <c r="Z245" s="1"/>
     </row>
-    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="s">
         <v>744</v>
       </c>
@@ -13042,7 +13045,9 @@
       <c r="H246" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="I246" s="5"/>
+      <c r="I246" s="4" t="s">
+        <v>752</v>
+      </c>
       <c r="J246" s="5"/>
       <c r="K246" s="5"/>
       <c r="L246" s="5"/>
@@ -13063,10 +13068,10 @@
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
@@ -13095,10 +13100,10 @@
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C248" s="3"/>
       <c r="D248" s="3"/>
@@ -13127,10 +13132,10 @@
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C249" s="3"/>
       <c r="D249" s="3"/>
@@ -13159,10 +13164,10 @@
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C250" s="3"/>
       <c r="D250" s="3"/>
@@ -13191,10 +13196,10 @@
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="3"/>
@@ -13223,10 +13228,10 @@
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="3"/>
@@ -13255,10 +13260,10 @@
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="3"/>
@@ -13287,10 +13292,10 @@
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="3"/>
@@ -13319,10 +13324,10 @@
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="3"/>
@@ -13351,10 +13356,10 @@
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C256" s="3"/>
       <c r="D256" s="3"/>
@@ -13383,10 +13388,10 @@
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="3"/>
@@ -13415,10 +13420,10 @@
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C258" s="3"/>
       <c r="D258" s="3"/>
@@ -13447,10 +13452,10 @@
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C259" s="3"/>
       <c r="D259" s="3"/>
@@ -13479,10 +13484,10 @@
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="3"/>
@@ -13511,10 +13516,10 @@
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C261" s="3"/>
       <c r="D261" s="3"/>
@@ -13543,10 +13548,10 @@
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C262" s="3"/>
       <c r="D262" s="3"/>
@@ -13575,10 +13580,10 @@
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C263" s="3"/>
       <c r="D263" s="3"/>
@@ -13607,10 +13612,10 @@
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C264" s="3"/>
       <c r="D264" s="3"/>
@@ -13639,10 +13644,10 @@
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C265" s="3"/>
       <c r="D265" s="3"/>
@@ -13671,10 +13676,10 @@
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C266" s="3"/>
       <c r="D266" s="3"/>
@@ -13703,10 +13708,10 @@
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C267" s="3"/>
       <c r="D267" s="3"/>
@@ -13735,10 +13740,10 @@
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C268" s="3"/>
       <c r="D268" s="3"/>
@@ -13767,10 +13772,10 @@
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C269" s="3"/>
       <c r="D269" s="3"/>
@@ -13799,10 +13804,10 @@
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C270" s="3"/>
       <c r="D270" s="3"/>
@@ -13831,10 +13836,10 @@
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C271" s="3"/>
       <c r="D271" s="3"/>
@@ -13863,10 +13868,10 @@
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C272" s="3"/>
       <c r="D272" s="3"/>
@@ -13895,10 +13900,10 @@
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C273" s="3"/>
       <c r="D273" s="3"/>
@@ -13927,10 +13932,10 @@
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C274" s="3"/>
       <c r="D274" s="3"/>
@@ -13959,10 +13964,10 @@
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C275" s="3"/>
       <c r="D275" s="3"/>
@@ -13991,10 +13996,10 @@
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="C276" s="3"/>
       <c r="D276" s="3"/>
@@ -14023,10 +14028,10 @@
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="C277" s="3"/>
       <c r="D277" s="3"/>
@@ -14055,10 +14060,10 @@
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C278" s="3"/>
       <c r="D278" s="3"/>
@@ -14087,10 +14092,10 @@
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C279" s="3"/>
       <c r="D279" s="3"/>
@@ -14119,10 +14124,10 @@
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C280" s="3"/>
       <c r="D280" s="3"/>
@@ -14151,10 +14156,10 @@
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C281" s="3"/>
       <c r="D281" s="3"/>
@@ -14183,10 +14188,10 @@
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C282" s="3"/>
       <c r="D282" s="3"/>
@@ -14215,10 +14220,10 @@
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C283" s="3"/>
       <c r="D283" s="3"/>
@@ -14247,10 +14252,10 @@
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C284" s="3"/>
       <c r="D284" s="3"/>
@@ -14279,10 +14284,10 @@
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C285" s="3"/>
       <c r="D285" s="3"/>
@@ -14311,10 +14316,10 @@
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C286" s="3"/>
       <c r="D286" s="3"/>
@@ -14343,10 +14348,10 @@
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C287" s="3"/>
       <c r="D287" s="3"/>
@@ -14375,10 +14380,10 @@
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C288" s="3"/>
       <c r="D288" s="3"/>
@@ -14407,10 +14412,10 @@
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C289" s="3"/>
       <c r="D289" s="3"/>
@@ -14439,10 +14444,10 @@
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C290" s="3"/>
       <c r="D290" s="3"/>
@@ -14471,10 +14476,10 @@
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C291" s="3"/>
       <c r="D291" s="3"/>
@@ -14503,10 +14508,10 @@
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C292" s="3"/>
       <c r="D292" s="3"/>
@@ -14535,10 +14540,10 @@
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C293" s="3"/>
       <c r="D293" s="3"/>
@@ -14567,10 +14572,10 @@
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C294" s="3"/>
       <c r="D294" s="3"/>
@@ -14599,10 +14604,10 @@
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C295" s="3"/>
       <c r="D295" s="3"/>
@@ -14631,10 +14636,10 @@
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C296" s="3"/>
       <c r="D296" s="3"/>
@@ -14663,10 +14668,10 @@
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C297" s="3"/>
       <c r="D297" s="3"/>
@@ -14695,10 +14700,10 @@
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C298" s="3"/>
       <c r="D298" s="3"/>
@@ -14727,10 +14732,10 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C299" s="3"/>
       <c r="D299" s="3"/>
@@ -14759,10 +14764,10 @@
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C300" s="3"/>
       <c r="D300" s="3"/>
@@ -14791,10 +14796,10 @@
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B301" s="3" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C301" s="3"/>
       <c r="D301" s="3"/>
@@ -14823,10 +14828,10 @@
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B302" s="3" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C302" s="3"/>
       <c r="D302" s="3"/>
@@ -14855,10 +14860,10 @@
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C303" s="3"/>
       <c r="D303" s="3"/>
@@ -14887,10 +14892,10 @@
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B304" s="3" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C304" s="3"/>
       <c r="D304" s="3"/>
@@ -14919,10 +14924,10 @@
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B305" s="3" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C305" s="3"/>
       <c r="D305" s="3"/>
@@ -14951,10 +14956,10 @@
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C306" s="3"/>
       <c r="D306" s="3"/>
@@ -14983,10 +14988,10 @@
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C307" s="3"/>
       <c r="D307" s="3"/>
@@ -15015,10 +15020,10 @@
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C308" s="3"/>
       <c r="D308" s="3"/>
@@ -15047,10 +15052,10 @@
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B309" s="3" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C309" s="3"/>
       <c r="D309" s="3"/>
@@ -15079,10 +15084,10 @@
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B310" s="3" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C310" s="3"/>
       <c r="D310" s="3"/>
@@ -15111,10 +15116,10 @@
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C311" s="3"/>
       <c r="D311" s="3"/>
@@ -15143,10 +15148,10 @@
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B312" s="3" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C312" s="3"/>
       <c r="D312" s="3"/>
@@ -15175,10 +15180,10 @@
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="2" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B313" s="3" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C313" s="3"/>
       <c r="D313" s="3"/>
@@ -15207,10 +15212,10 @@
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B314" s="3" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C314" s="3"/>
       <c r="D314" s="3"/>
@@ -15239,10 +15244,10 @@
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B315" s="3" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C315" s="3"/>
       <c r="D315" s="3"/>
@@ -15271,10 +15276,10 @@
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B316" s="3" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
@@ -15303,10 +15308,10 @@
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B317" s="3" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C317" s="3"/>
       <c r="D317" s="3"/>
@@ -15335,10 +15340,10 @@
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B318" s="3" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C318" s="3"/>
       <c r="D318" s="3"/>
@@ -15367,10 +15372,10 @@
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C319" s="3"/>
       <c r="D319" s="3"/>
@@ -15399,10 +15404,10 @@
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C320" s="3"/>
       <c r="D320" s="3"/>
@@ -15431,10 +15436,10 @@
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B321" s="3" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C321" s="3"/>
       <c r="D321" s="3"/>
@@ -15463,10 +15468,10 @@
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C322" s="3"/>
       <c r="D322" s="3"/>
@@ -15495,10 +15500,10 @@
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C323" s="3"/>
       <c r="D323" s="3"/>
@@ -15527,10 +15532,10 @@
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B324" s="3" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C324" s="3"/>
       <c r="D324" s="3"/>
@@ -15559,10 +15564,10 @@
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B325" s="3" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C325" s="3"/>
       <c r="D325" s="3"/>
@@ -15591,10 +15596,10 @@
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="B326" s="3" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C326" s="3"/>
       <c r="D326" s="3"/>
@@ -15623,10 +15628,10 @@
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="B327" s="3" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C327" s="3"/>
       <c r="D327" s="3"/>
@@ -15655,10 +15660,10 @@
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="2" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B328" s="3" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C328" s="3"/>
       <c r="D328" s="3"/>
@@ -15687,10 +15692,10 @@
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="2" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B329" s="3" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C329" s="3"/>
       <c r="D329" s="3"/>
@@ -15719,10 +15724,10 @@
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C330" s="3"/>
       <c r="D330" s="3"/>
@@ -15751,10 +15756,10 @@
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C331" s="3"/>
       <c r="D331" s="3"/>
@@ -15783,10 +15788,10 @@
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C332" s="3"/>
       <c r="D332" s="3"/>
@@ -15815,10 +15820,10 @@
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C333" s="3"/>
       <c r="D333" s="3"/>
@@ -15847,10 +15852,10 @@
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C334" s="3"/>
       <c r="D334" s="3"/>
@@ -15879,10 +15884,10 @@
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C335" s="3"/>
       <c r="D335" s="3"/>
@@ -15911,10 +15916,10 @@
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C336" s="3"/>
       <c r="D336" s="3"/>
@@ -15943,10 +15948,10 @@
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C337" s="3"/>
       <c r="D337" s="3"/>
@@ -15975,10 +15980,10 @@
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C338" s="3"/>
       <c r="D338" s="3"/>
@@ -16007,10 +16012,10 @@
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C339" s="3"/>
       <c r="D339" s="3"/>
@@ -16039,10 +16044,10 @@
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C340" s="3"/>
       <c r="D340" s="3"/>
@@ -16071,10 +16076,10 @@
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B341" s="3" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C341" s="3"/>
       <c r="D341" s="3"/>
@@ -16103,10 +16108,10 @@
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B342" s="3" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C342" s="3"/>
       <c r="D342" s="3"/>
@@ -16135,10 +16140,10 @@
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C343" s="3"/>
       <c r="D343" s="3"/>
@@ -16167,10 +16172,10 @@
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C344" s="3"/>
       <c r="D344" s="3"/>
@@ -16199,10 +16204,10 @@
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C345" s="3"/>
       <c r="D345" s="3"/>
@@ -16231,10 +16236,10 @@
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C346" s="3"/>
       <c r="D346" s="3"/>
@@ -16263,10 +16268,10 @@
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B347" s="3" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C347" s="3"/>
       <c r="D347" s="3"/>
@@ -16295,10 +16300,10 @@
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C348" s="3"/>
       <c r="D348" s="3"/>
@@ -16327,10 +16332,10 @@
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B349" s="3" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C349" s="3"/>
       <c r="D349" s="3"/>
@@ -16359,10 +16364,10 @@
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="C350" s="3"/>
       <c r="D350" s="3"/>
@@ -16391,10 +16396,10 @@
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B351" s="3" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C351" s="3"/>
       <c r="D351" s="3"/>
@@ -16423,10 +16428,10 @@
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C352" s="3"/>
       <c r="D352" s="3"/>
@@ -16455,10 +16460,10 @@
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C353" s="3"/>
       <c r="D353" s="3"/>
@@ -16487,10 +16492,10 @@
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="2" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C354" s="3"/>
       <c r="D354" s="3"/>
@@ -16519,10 +16524,10 @@
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C355" s="3"/>
       <c r="D355" s="3"/>
@@ -16551,10 +16556,10 @@
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C356" s="3"/>
       <c r="D356" s="3"/>
@@ -16583,10 +16588,10 @@
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C357" s="3"/>
       <c r="D357" s="3"/>
@@ -16615,10 +16620,10 @@
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C358" s="3"/>
       <c r="D358" s="3"/>
@@ -16647,10 +16652,10 @@
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C359" s="3"/>
       <c r="D359" s="3"/>
@@ -16679,10 +16684,10 @@
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B360" s="3" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C360" s="3"/>
       <c r="D360" s="3"/>
@@ -16711,10 +16716,10 @@
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C361" s="3"/>
       <c r="D361" s="3"/>
@@ -16743,10 +16748,10 @@
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C362" s="3"/>
       <c r="D362" s="3"/>
@@ -16775,10 +16780,10 @@
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C363" s="3"/>
       <c r="D363" s="3"/>
@@ -16807,10 +16812,10 @@
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="C364" s="3"/>
       <c r="D364" s="3"/>
@@ -16839,10 +16844,10 @@
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C365" s="3"/>
       <c r="D365" s="3"/>
@@ -16871,10 +16876,10 @@
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C366" s="3"/>
       <c r="D366" s="3"/>
@@ -16903,10 +16908,10 @@
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C367" s="3"/>
       <c r="D367" s="3"/>
@@ -16935,10 +16940,10 @@
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="C368" s="3"/>
       <c r="D368" s="3"/>
@@ -16967,10 +16972,10 @@
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C369" s="3"/>
       <c r="D369" s="3"/>
@@ -16999,10 +17004,10 @@
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="2" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C370" s="3"/>
       <c r="D370" s="3"/>
@@ -17031,10 +17036,10 @@
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="2" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B371" s="3" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="C371" s="3"/>
       <c r="D371" s="3"/>
@@ -17063,10 +17068,10 @@
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="2" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B372" s="3" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C372" s="3"/>
       <c r="D372" s="3"/>
@@ -17095,10 +17100,10 @@
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B373" s="3" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C373" s="3"/>
       <c r="D373" s="3"/>
@@ -17127,10 +17132,10 @@
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C374" s="3"/>
       <c r="D374" s="3"/>
@@ -17159,10 +17164,10 @@
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C375" s="3"/>
       <c r="D375" s="3"/>
@@ -17191,10 +17196,10 @@
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B376" s="3" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C376" s="3"/>
       <c r="D376" s="3"/>
@@ -17223,10 +17228,10 @@
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="2" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C377" s="3"/>
       <c r="D377" s="3"/>
@@ -17255,10 +17260,10 @@
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C378" s="3"/>
       <c r="D378" s="3"/>
@@ -17287,10 +17292,10 @@
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="C379" s="3"/>
       <c r="D379" s="3"/>
@@ -17319,10 +17324,10 @@
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C380" s="3"/>
       <c r="D380" s="3"/>
@@ -17351,10 +17356,10 @@
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B381" s="3" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C381" s="3"/>
       <c r="D381" s="3"/>
@@ -17383,10 +17388,10 @@
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B382" s="3" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="C382" s="3"/>
       <c r="D382" s="3"/>
@@ -17415,10 +17420,10 @@
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B383" s="3" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C383" s="3"/>
       <c r="D383" s="3"/>
@@ -17447,10 +17452,10 @@
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B384" s="3" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C384" s="3"/>
       <c r="D384" s="3"/>
@@ -17479,10 +17484,10 @@
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B385" s="3" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C385" s="3"/>
       <c r="D385" s="3"/>
@@ -17511,10 +17516,10 @@
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B386" s="3" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C386" s="3"/>
       <c r="D386" s="3"/>
@@ -17543,10 +17548,10 @@
     </row>
     <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B387" s="3" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C387" s="3"/>
       <c r="D387" s="3"/>
@@ -17575,10 +17580,10 @@
     </row>
     <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B388" s="3" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C388" s="3"/>
       <c r="D388" s="3"/>
@@ -17607,10 +17612,10 @@
     </row>
     <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C389" s="3"/>
       <c r="D389" s="3"/>
@@ -17639,10 +17644,10 @@
     </row>
     <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C390" s="3"/>
       <c r="D390" s="3"/>
@@ -17671,10 +17676,10 @@
     </row>
     <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C391" s="3"/>
       <c r="D391" s="3"/>
@@ -17703,10 +17708,10 @@
     </row>
     <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="2" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C392" s="3"/>
       <c r="D392" s="3"/>
@@ -17735,10 +17740,10 @@
     </row>
     <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="2" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C393" s="3"/>
       <c r="D393" s="3"/>
@@ -17767,10 +17772,10 @@
     </row>
     <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="2" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="C394" s="3"/>
       <c r="D394" s="3"/>
@@ -17799,10 +17804,10 @@
     </row>
     <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="2" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C395" s="3"/>
       <c r="D395" s="3"/>
@@ -17831,10 +17836,10 @@
     </row>
     <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="2" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C396" s="3"/>
       <c r="D396" s="3"/>
@@ -17863,10 +17868,10 @@
     </row>
     <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="C397" s="3"/>
       <c r="D397" s="3"/>
@@ -17895,10 +17900,10 @@
     </row>
     <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="C398" s="3"/>
       <c r="D398" s="3"/>
@@ -17927,10 +17932,10 @@
     </row>
     <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="C399" s="3"/>
       <c r="D399" s="3"/>
@@ -17959,10 +17964,10 @@
     </row>
     <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="2" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C400" s="3"/>
       <c r="D400" s="3"/>
@@ -17991,10 +17996,10 @@
     </row>
     <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="2" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="C401" s="3"/>
       <c r="D401" s="3"/>
@@ -18023,10 +18028,10 @@
     </row>
     <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="2" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C402" s="3"/>
       <c r="D402" s="3"/>
@@ -18055,10 +18060,10 @@
     </row>
     <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="C403" s="3"/>
       <c r="D403" s="3"/>
@@ -18087,10 +18092,10 @@
     </row>
     <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="2" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C404" s="3"/>
       <c r="D404" s="3"/>
@@ -18119,10 +18124,10 @@
     </row>
     <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="2" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C405" s="3"/>
       <c r="D405" s="3"/>
@@ -18151,10 +18156,10 @@
     </row>
     <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="2" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="C406" s="3"/>
       <c r="D406" s="3"/>
@@ -18183,10 +18188,10 @@
     </row>
     <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="2" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="C407" s="3"/>
       <c r="D407" s="3"/>
@@ -18215,10 +18220,10 @@
     </row>
     <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="2" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C408" s="3"/>
       <c r="D408" s="3"/>
@@ -18247,10 +18252,10 @@
     </row>
     <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="2" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C409" s="3"/>
       <c r="D409" s="3"/>
@@ -18279,10 +18284,10 @@
     </row>
     <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="2" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C410" s="3"/>
       <c r="D410" s="3"/>
@@ -18311,10 +18316,10 @@
     </row>
     <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="2" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C411" s="3"/>
       <c r="D411" s="3"/>
@@ -18343,10 +18348,10 @@
     </row>
     <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="2" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C412" s="3"/>
       <c r="D412" s="3"/>
@@ -18375,10 +18380,10 @@
     </row>
     <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="2" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C413" s="3"/>
       <c r="D413" s="3"/>
@@ -18407,10 +18412,10 @@
     </row>
     <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="2" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C414" s="3"/>
       <c r="D414" s="3"/>
@@ -18439,10 +18444,10 @@
     </row>
     <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="2" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C415" s="3"/>
       <c r="D415" s="3"/>
@@ -18471,10 +18476,10 @@
     </row>
     <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="2" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C416" s="3"/>
       <c r="D416" s="3"/>
@@ -18503,10 +18508,10 @@
     </row>
     <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="2" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C417" s="3"/>
       <c r="D417" s="3"/>
@@ -18535,10 +18540,10 @@
     </row>
     <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="2" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C418" s="3"/>
       <c r="D418" s="3"/>
@@ -18567,10 +18572,10 @@
     </row>
     <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="2" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C419" s="3"/>
       <c r="D419" s="3"/>
@@ -18599,10 +18604,10 @@
     </row>
     <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C420" s="3"/>
       <c r="D420" s="3"/>
@@ -18631,10 +18636,10 @@
     </row>
     <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="C421" s="3"/>
       <c r="D421" s="3"/>
@@ -18663,10 +18668,10 @@
     </row>
     <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B422" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C422" s="3"/>
       <c r="D422" s="3"/>
@@ -18695,10 +18700,10 @@
     </row>
     <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="2" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C423" s="3"/>
       <c r="D423" s="3"/>
@@ -18727,10 +18732,10 @@
     </row>
     <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C424" s="3"/>
       <c r="D424" s="3"/>
@@ -18759,10 +18764,10 @@
     </row>
     <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C425" s="3"/>
       <c r="D425" s="3"/>
@@ -18791,10 +18796,10 @@
     </row>
     <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C426" s="3"/>
       <c r="D426" s="3"/>
@@ -18823,10 +18828,10 @@
     </row>
     <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C427" s="3"/>
       <c r="D427" s="3"/>
@@ -18855,10 +18860,10 @@
     </row>
     <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C428" s="3"/>
       <c r="D428" s="3"/>
@@ -18887,10 +18892,10 @@
     </row>
     <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="2" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B429" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C429" s="3"/>
       <c r="D429" s="3"/>
@@ -18919,10 +18924,10 @@
     </row>
     <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C430" s="3"/>
       <c r="D430" s="3"/>
@@ -18951,10 +18956,10 @@
     </row>
     <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C431" s="3"/>
       <c r="D431" s="3"/>
@@ -18983,10 +18988,10 @@
     </row>
     <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="C432" s="3"/>
       <c r="D432" s="3"/>
@@ -19015,10 +19020,10 @@
     </row>
     <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -19047,10 +19052,10 @@
     </row>
     <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -19079,10 +19084,10 @@
     </row>
     <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="C435" s="3"/>
       <c r="D435" s="3"/>
@@ -19111,10 +19116,10 @@
     </row>
     <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C436" s="3"/>
       <c r="D436" s="3"/>
@@ -19143,10 +19148,10 @@
     </row>
     <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C437" s="3"/>
       <c r="D437" s="3"/>
@@ -19175,10 +19180,10 @@
     </row>
     <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C438" s="3"/>
       <c r="D438" s="3"/>
@@ -19207,10 +19212,10 @@
     </row>
     <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="C439" s="3"/>
       <c r="D439" s="3"/>
@@ -19239,10 +19244,10 @@
     </row>
     <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="C440" s="3"/>
       <c r="D440" s="3"/>
@@ -19271,10 +19276,10 @@
     </row>
     <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C441" s="3"/>
       <c r="D441" s="3"/>
@@ -19303,10 +19308,10 @@
     </row>
     <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C442" s="3"/>
       <c r="D442" s="3"/>
@@ -19335,10 +19340,10 @@
     </row>
     <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C443" s="3"/>
       <c r="D443" s="3"/>
@@ -19367,10 +19372,10 @@
     </row>
     <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C444" s="3"/>
       <c r="D444" s="3"/>
@@ -19399,10 +19404,10 @@
     </row>
     <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="C445" s="3"/>
       <c r="D445" s="3"/>
@@ -19431,10 +19436,10 @@
     </row>
     <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="C446" s="3"/>
       <c r="D446" s="3"/>
@@ -19463,7 +19468,7 @@
     </row>
     <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B447" s="5"/>
       <c r="C447" s="5"/>
@@ -19493,7 +19498,7 @@
     </row>
     <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="B448" s="5"/>
       <c r="C448" s="5"/>
@@ -19523,7 +19528,7 @@
     </row>
     <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="B449" s="5"/>
       <c r="C449" s="5"/>
@@ -19553,10 +19558,10 @@
     </row>
     <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="B450" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C450" s="3"/>
       <c r="D450" s="3"/>
@@ -19585,10 +19590,10 @@
     </row>
     <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B451" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="C451" s="3"/>
       <c r="D451" s="3"/>
@@ -19617,10 +19622,10 @@
     </row>
     <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="B452" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="C452" s="3"/>
       <c r="D452" s="3"/>
@@ -19649,10 +19654,10 @@
     </row>
     <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="B453" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="C453" s="3"/>
       <c r="D453" s="3"/>
@@ -19681,10 +19686,10 @@
     </row>
     <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="B454" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C454" s="3"/>
       <c r="D454" s="3"/>
@@ -19713,10 +19718,10 @@
     </row>
     <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="B455" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C455" s="3"/>
       <c r="D455" s="3"/>
@@ -19745,10 +19750,10 @@
     </row>
     <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="B456" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="C456" s="3"/>
       <c r="D456" s="3"/>
@@ -19777,10 +19782,10 @@
     </row>
     <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B457" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="C457" s="3"/>
       <c r="D457" s="3"/>
@@ -19809,10 +19814,10 @@
     </row>
     <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="B458" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="C458" s="3"/>
       <c r="D458" s="3"/>
@@ -19841,10 +19846,10 @@
     </row>
     <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B459" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="C459" s="3"/>
       <c r="D459" s="3"/>
@@ -19873,10 +19878,10 @@
     </row>
     <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="B460" s="3" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="C460" s="3"/>
       <c r="D460" s="3"/>
@@ -19905,10 +19910,10 @@
     </row>
     <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="B461" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="C461" s="3"/>
       <c r="D461" s="3"/>
@@ -19937,10 +19942,10 @@
     </row>
     <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="B462" s="3" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="C462" s="3"/>
       <c r="D462" s="3"/>
@@ -19969,10 +19974,10 @@
     </row>
     <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="B463" s="3" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="C463" s="3"/>
       <c r="D463" s="3"/>
@@ -20001,10 +20006,10 @@
     </row>
     <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="B464" s="3" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="C464" s="3"/>
       <c r="D464" s="3"/>
@@ -20033,10 +20038,10 @@
     </row>
     <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="B465" s="3" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="C465" s="3"/>
       <c r="D465" s="3"/>
@@ -20065,7 +20070,7 @@
     </row>
     <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="2" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="B466" s="5"/>
       <c r="C466" s="5"/>
@@ -20095,7 +20100,7 @@
     </row>
     <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="2" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B467" s="5"/>
       <c r="C467" s="5"/>
@@ -20125,7 +20130,7 @@
     </row>
     <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="B468" s="5"/>
       <c r="C468" s="5"/>
@@ -20155,7 +20160,7 @@
     </row>
     <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B469" s="5"/>
       <c r="C469" s="5"/>
@@ -20185,7 +20190,7 @@
     </row>
     <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="2" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="B470" s="5"/>
       <c r="C470" s="5"/>
@@ -20215,7 +20220,7 @@
     </row>
     <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B471" s="5"/>
       <c r="C471" s="5"/>
@@ -20245,7 +20250,7 @@
     </row>
     <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="2" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="B472" s="5"/>
       <c r="C472" s="5"/>
@@ -20275,7 +20280,7 @@
     </row>
     <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B473" s="5"/>
       <c r="C473" s="5"/>
@@ -20305,7 +20310,7 @@
     </row>
     <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="B474" s="5"/>
       <c r="C474" s="5"/>
@@ -20335,7 +20340,7 @@
     </row>
     <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="2" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B475" s="5"/>
       <c r="C475" s="5"/>
@@ -20365,7 +20370,7 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B476" s="5"/>
       <c r="C476" s="5"/>
@@ -20395,7 +20400,7 @@
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B477" s="5"/>
       <c r="C477" s="5"/>
@@ -20425,7 +20430,7 @@
     </row>
     <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="2" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B478" s="5"/>
       <c r="C478" s="5"/>
@@ -20455,7 +20460,7 @@
     </row>
     <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B479" s="5"/>
       <c r="C479" s="5"/>
@@ -20485,7 +20490,7 @@
     </row>
     <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="B480" s="5"/>
       <c r="C480" s="5"/>
@@ -20515,7 +20520,7 @@
     </row>
     <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="B481" s="5"/>
       <c r="C481" s="5"/>
@@ -20553,7 +20558,7 @@
       <c r="G482" s="14"/>
       <c r="H482" s="14"/>
       <c r="I482" s="3" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="J482" s="3"/>
       <c r="K482" s="14"/>
@@ -20575,37 +20580,37 @@
     </row>
     <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="E483" s="4" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="F483" s="4" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="G483" s="4" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="H483" s="4" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="I483" s="4" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="J483" s="4" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="K483" s="4" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="L483" s="5"/>
       <c r="M483" s="5"/>
@@ -20625,37 +20630,37 @@
     </row>
     <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B484" s="4" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="D484" s="4" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F484" s="4" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="G484" s="4" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="H484" s="4" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="I484" s="4" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="J484" s="4" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="K484" s="4" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="L484" s="5"/>
       <c r="M484" s="5"/>
@@ -20675,37 +20680,37 @@
     </row>
     <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="E485" s="4" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="F485" s="4" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="G485" s="4" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="H485" s="4" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="I485" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="J485" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="K485" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="L485" s="5"/>
       <c r="M485" s="5"/>
@@ -20725,37 +20730,37 @@
     </row>
     <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="B486" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D486" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="E486" s="4" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="F486" s="4" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="G486" s="4" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="H486" s="4" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="I486" s="4" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="J486" s="4" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="K486" s="4" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="L486" s="5"/>
       <c r="M486" s="5"/>
@@ -20775,37 +20780,37 @@
     </row>
     <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="E487" s="4" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="F487" s="4" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="G487" s="4" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="H487" s="4" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="I487" s="4" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="J487" s="4" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="K487" s="4" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="L487" s="5"/>
       <c r="M487" s="5"/>
@@ -20825,37 +20830,37 @@
     </row>
     <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="B488" s="4" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D488" s="4" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="F488" s="4" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="G488" s="4" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="H488" s="4" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="I488" s="4" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="J488" s="4" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="K488" s="4" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="L488" s="5"/>
       <c r="M488" s="5"/>
@@ -20875,37 +20880,37 @@
     </row>
     <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="F489" s="4" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="G489" s="4" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="H489" s="4" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="I489" s="4" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="J489" s="4" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="K489" s="4" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="L489" s="5"/>
       <c r="M489" s="5"/>
@@ -20925,37 +20930,37 @@
     </row>
     <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="F490" s="4" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="G490" s="4" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="H490" s="4" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="I490" s="4" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="J490" s="4" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="K490" s="4" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="L490" s="5"/>
       <c r="M490" s="5"/>
@@ -20975,37 +20980,37 @@
     </row>
     <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
       <c r="E491" s="4" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="F491" s="4" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="G491" s="4" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
       <c r="H491" s="4" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
       <c r="I491" s="4" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
       <c r="J491" s="4" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="K491" s="4" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="L491" s="5"/>
       <c r="M491" s="5"/>
@@ -21025,37 +21030,37 @@
     </row>
     <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="F492" s="4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
       <c r="G492" s="4" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="H492" s="4" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="I492" s="4" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="J492" s="4" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
       <c r="K492" s="4" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="L492" s="5"/>
       <c r="M492" s="5"/>
@@ -21075,37 +21080,37 @@
     </row>
     <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="B493" s="4" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
       <c r="E493" s="4" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="F493" s="4" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="G493" s="4" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="H493" s="4" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="I493" s="4" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="J493" s="4" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="K493" s="4" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="L493" s="5"/>
       <c r="M493" s="5"/>
@@ -21125,37 +21130,37 @@
     </row>
     <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="E494" s="4" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="F494" s="4" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="G494" s="4" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="H494" s="4" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="I494" s="4" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="J494" s="4" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="K494" s="4" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="L494" s="5"/>
       <c r="M494" s="5"/>
@@ -21175,38 +21180,38 @@
     </row>
     <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="C495" s="3"/>
       <c r="D495" s="3" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="E495" s="3"/>
       <c r="F495" s="3" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="G495" s="3"/>
       <c r="H495" s="3" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="I495" s="3"/>
       <c r="J495" s="3" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="K495" s="3"/>
       <c r="L495" s="3" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="M495" s="3"/>
       <c r="N495" s="3" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
       <c r="O495" s="3"/>
       <c r="P495" s="3" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="Q495" s="3"/>
       <c r="R495" s="1"/>
@@ -21221,34 +21226,34 @@
     </row>
     <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="F496" s="4" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="G496" s="4" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="H496" s="4" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="I496" s="4" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="J496" s="4" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="K496" s="5"/>
       <c r="L496" s="5"/>
@@ -21269,34 +21274,34 @@
     </row>
     <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="E497" s="4" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="F497" s="4" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="G497" s="4" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="H497" s="4" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
       <c r="I497" s="4" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="J497" s="4" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="K497" s="5"/>
       <c r="L497" s="5"/>
@@ -21317,34 +21322,34 @@
     </row>
     <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
       <c r="F498" s="4" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="G498" s="4" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="H498" s="4" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
       <c r="I498" s="4" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
       <c r="J498" s="4" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="K498" s="5"/>
       <c r="L498" s="5"/>
@@ -21365,34 +21370,34 @@
     </row>
     <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="B499" s="4" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="F499" s="4" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="G499" s="4" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="H499" s="4" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="I499" s="4" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="J499" s="4" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="K499" s="5"/>
       <c r="L499" s="5"/>
@@ -21413,34 +21418,34 @@
     </row>
     <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="2" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="F500" s="4" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="G500" s="4" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="H500" s="4" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="I500" s="4" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="J500" s="4" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="K500" s="5"/>
       <c r="L500" s="5"/>
@@ -21461,34 +21466,34 @@
     </row>
     <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="2" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="C501" s="4" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="E501" s="4" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="F501" s="4" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="G501" s="4" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="H501" s="4" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="I501" s="4" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="J501" s="4" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="K501" s="5"/>
       <c r="L501" s="5"/>
@@ -21509,34 +21514,34 @@
     </row>
     <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="2" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="B502" s="4" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="C502" s="4" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="D502" s="4" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="E502" s="4" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="F502" s="4" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="G502" s="4" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="H502" s="4" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="I502" s="4" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="J502" s="4" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="K502" s="5"/>
       <c r="L502" s="5"/>
@@ -21557,30 +21562,30 @@
     </row>
     <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="2" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="C503" s="3"/>
       <c r="D503" s="3" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="E503" s="3"/>
       <c r="F503" s="3" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="G503" s="3"/>
       <c r="H503" s="3" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="I503" s="3"/>
       <c r="J503" s="3" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="K503" s="3"/>
       <c r="L503" s="3" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="M503" s="3"/>
       <c r="N503" s="5"/>
@@ -21599,38 +21604,38 @@
     </row>
     <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="2" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="B504" s="3" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="C504" s="3"/>
       <c r="D504" s="3" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="E504" s="3"/>
       <c r="F504" s="3" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="G504" s="3"/>
       <c r="H504" s="3" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="I504" s="3"/>
       <c r="J504" s="3" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="K504" s="3"/>
       <c r="L504" s="3" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="M504" s="3"/>
       <c r="N504" s="3" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="O504" s="3"/>
       <c r="P504" s="3" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="Q504" s="3"/>
       <c r="R504" s="1"/>
@@ -21645,14 +21650,14 @@
     </row>
     <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="2" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="B505" s="3" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="C505" s="3"/>
       <c r="D505" s="3" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="E505" s="3"/>
       <c r="F505" s="5"/>
@@ -21660,19 +21665,19 @@
       <c r="H505" s="5"/>
       <c r="I505" s="5"/>
       <c r="J505" s="3" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="K505" s="3"/>
       <c r="L505" s="3" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="M505" s="3"/>
       <c r="N505" s="3" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="O505" s="3"/>
       <c r="P505" s="3" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="Q505" s="3"/>
       <c r="R505" s="1"/>
@@ -21687,30 +21692,30 @@
     </row>
     <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="2" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="B506" s="3" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="C506" s="3"/>
       <c r="D506" s="3" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="E506" s="3"/>
       <c r="F506" s="3" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="G506" s="3"/>
       <c r="H506" s="3" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="I506" s="3"/>
       <c r="J506" s="3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="K506" s="3"/>
       <c r="L506" s="3" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="M506" s="3"/>
       <c r="N506" s="5"/>
@@ -21729,28 +21734,28 @@
     </row>
     <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="2" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="B507" s="4" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="D507" s="4" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="E507" s="4" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="F507" s="4" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="G507" s="5"/>
       <c r="H507" s="5"/>
       <c r="I507" s="5"/>
       <c r="J507" s="3" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="K507" s="3"/>
       <c r="L507" s="5"/>
@@ -21758,10 +21763,10 @@
       <c r="N507" s="5"/>
       <c r="O507" s="5"/>
       <c r="P507" s="4" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="Q507" s="4" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="R507" s="1"/>
       <c r="S507" s="1"/>
@@ -21775,7 +21780,7 @@
     </row>
     <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="2" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B508" s="5"/>
       <c r="C508" s="5"/>
@@ -21805,7 +21810,7 @@
     </row>
     <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="2" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B509" s="5"/>
       <c r="C509" s="5"/>
@@ -21835,7 +21840,7 @@
     </row>
     <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="2" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B510" s="5"/>
       <c r="C510" s="5"/>
@@ -21865,7 +21870,7 @@
     </row>
     <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="2" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B511" s="5"/>
       <c r="C511" s="5"/>
@@ -21895,7 +21900,7 @@
     </row>
     <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="2" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="B512" s="5"/>
       <c r="C512" s="5"/>
@@ -21925,7 +21930,7 @@
     </row>
     <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="2" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="B513" s="5"/>
       <c r="C513" s="5"/>
@@ -21955,7 +21960,7 @@
     </row>
     <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="2" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="B514" s="5"/>
       <c r="C514" s="5"/>

</xml_diff>